<commit_message>
Update to python capabilities, it can now update Language, Relation to Itera, Domain, Practice, Tags and Synonyms. Also Adding a "name to ID" file to make writing practices in excel easier.
</commit_message>
<xml_diff>
--- a/Excel_to_Sanity_Importation/Glossary compilations.xlsx
+++ b/Excel_to_Sanity_Importation/Glossary compilations.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hakon.bolviken\Documents\GitHub\level-up-sanity\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hakon.bolviken\Documents\GitHub\level-up-sanity\Excel_to_Sanity_Importation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC82512E-724A-4C2C-8B0F-2DA0525E1C50}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE350887-F945-44EB-A313-F93761D85490}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Excel" sheetId="1" r:id="rId1"/>
@@ -52,7 +52,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="628" uniqueCount="564">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="625" uniqueCount="570">
   <si>
     <t>Long hand</t>
   </si>
@@ -2003,16 +2003,34 @@
     <t>ICNO</t>
   </si>
   <si>
+    <t>ID</t>
+  </si>
+  <si>
+    <t>Integration developer</t>
+  </si>
+  <si>
+    <t>Programmer coding back-end applications (server-side)</t>
+  </si>
+  <si>
+    <t>Related to Practice</t>
+  </si>
+  <si>
+    <t>Related to Itera</t>
+  </si>
+  <si>
     <t>Itera Consulting NO?</t>
   </si>
   <si>
-    <t>ID</t>
-  </si>
-  <si>
-    <t>Integration developer</t>
-  </si>
-  <si>
-    <t>Programmer coding back-end applications (server-side)</t>
+    <t>Language</t>
+  </si>
+  <si>
+    <t>Related to Domain</t>
+  </si>
+  <si>
+    <t>Tags</t>
+  </si>
+  <si>
+    <t>Synonyms</t>
   </si>
 </sst>
 </file>
@@ -2406,10 +2424,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C298"/>
+  <dimension ref="A1:D298"/>
   <sheetViews>
-    <sheetView topLeftCell="A47" workbookViewId="0">
-      <selection activeCell="C262" sqref="C262"/>
+    <sheetView topLeftCell="B166" workbookViewId="0">
+      <selection activeCell="C177" sqref="C177"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2420,7 +2438,7 @@
     <col min="4" max="16384" width="9.109375" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>429</v>
       </c>
@@ -2430,1413 +2448,2120 @@
       <c r="C1" s="2" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D1" s="2" t="s">
+        <v>560</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>2</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D2" s="2">
+        <f>4000</f>
+        <v>4000</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>4</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D3" s="2">
+        <f>D2+1</f>
+        <v>4001</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>6</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="D4" s="2">
+        <f t="shared" ref="D4:D67" si="0">D3+1</f>
+        <v>4002</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>8</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D5" s="2">
+        <f t="shared" si="0"/>
+        <v>4003</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>10</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D6" s="2">
+        <f t="shared" si="0"/>
+        <v>4004</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>12</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D7" s="2">
+        <f t="shared" si="0"/>
+        <v>4005</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>14</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="D8" s="2">
+        <f t="shared" si="0"/>
+        <v>4006</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>16</v>
       </c>
       <c r="C9" s="3" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="D9" s="2">
+        <f t="shared" si="0"/>
+        <v>4007</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>18</v>
       </c>
       <c r="C10" s="3" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="D10" s="2">
+        <f t="shared" si="0"/>
+        <v>4008</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>20</v>
       </c>
       <c r="C11" s="3" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D11" s="2">
+        <f t="shared" si="0"/>
+        <v>4009</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
         <v>22</v>
       </c>
       <c r="C12" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D12" s="2">
+        <f t="shared" si="0"/>
+        <v>4010</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
         <v>24</v>
       </c>
       <c r="C13" s="2" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D13" s="2">
+        <f t="shared" si="0"/>
+        <v>4011</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
         <v>26</v>
       </c>
       <c r="C14" s="2" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D14" s="2">
+        <f t="shared" si="0"/>
+        <v>4012</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
         <v>28</v>
       </c>
       <c r="C15" s="2" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D15" s="2">
+        <f t="shared" si="0"/>
+        <v>4013</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
         <v>30</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D16" s="2">
+        <f t="shared" si="0"/>
+        <v>4014</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
         <v>32</v>
       </c>
       <c r="C17" s="2" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D17" s="2">
+        <f t="shared" si="0"/>
+        <v>4015</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
         <v>34</v>
       </c>
       <c r="C18" s="2" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="D18" s="2">
+        <f t="shared" si="0"/>
+        <v>4016</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
         <v>36</v>
       </c>
       <c r="C19" s="3" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D19" s="2">
+        <f t="shared" si="0"/>
+        <v>4017</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
         <v>38</v>
       </c>
       <c r="C20" s="2" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D20" s="2">
+        <f t="shared" si="0"/>
+        <v>4018</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
         <v>40</v>
       </c>
       <c r="C21" s="2" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D21" s="2">
+        <f t="shared" si="0"/>
+        <v>4019</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
         <v>42</v>
       </c>
       <c r="C22" s="2" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D22" s="2">
+        <f t="shared" si="0"/>
+        <v>4020</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
         <v>44</v>
       </c>
       <c r="C23" s="2" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D23" s="2">
+        <f t="shared" si="0"/>
+        <v>4021</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24" s="2" t="s">
         <v>46</v>
       </c>
       <c r="C24" s="2" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D24" s="2">
+        <f t="shared" si="0"/>
+        <v>4022</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25" s="2" t="s">
         <v>48</v>
       </c>
       <c r="C25" s="2" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D25" s="2">
+        <f t="shared" si="0"/>
+        <v>4023</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26" s="2" t="s">
         <v>50</v>
       </c>
       <c r="C26" s="2" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D26" s="2">
+        <f t="shared" si="0"/>
+        <v>4024</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27" s="2" t="s">
         <v>52</v>
       </c>
       <c r="C27" s="2" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="28" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="D27" s="2">
+        <f t="shared" si="0"/>
+        <v>4025</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A28" s="2" t="s">
         <v>54</v>
       </c>
       <c r="C28" s="3" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D28" s="2">
+        <f t="shared" si="0"/>
+        <v>4026</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A29" s="2" t="s">
         <v>56</v>
       </c>
       <c r="C29" s="2" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D29" s="2">
+        <f t="shared" si="0"/>
+        <v>4027</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A30" s="2" t="s">
         <v>58</v>
       </c>
       <c r="C30" s="2" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D30" s="2">
+        <f t="shared" si="0"/>
+        <v>4028</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A31" s="2" t="s">
         <v>60</v>
       </c>
       <c r="C31" s="2" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D31" s="2">
+        <f t="shared" si="0"/>
+        <v>4029</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A32" s="2" t="s">
         <v>62</v>
       </c>
       <c r="C32" s="2" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="33" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="D32" s="2">
+        <f t="shared" si="0"/>
+        <v>4030</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A33" s="2" t="s">
         <v>64</v>
       </c>
       <c r="C33" s="3" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D33" s="2">
+        <f t="shared" si="0"/>
+        <v>4031</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A34" s="2" t="s">
         <v>66</v>
       </c>
       <c r="C34" s="2" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D34" s="2">
+        <f t="shared" si="0"/>
+        <v>4032</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A35" s="2" t="s">
         <v>68</v>
       </c>
       <c r="C35" s="2" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D35" s="2">
+        <f t="shared" si="0"/>
+        <v>4033</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A36" s="2" t="s">
         <v>70</v>
       </c>
       <c r="C36" s="2" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D36" s="2">
+        <f t="shared" si="0"/>
+        <v>4034</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A37" s="2" t="s">
         <v>72</v>
       </c>
       <c r="C37" s="2" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="38" spans="1:3" ht="72" x14ac:dyDescent="0.3">
+      <c r="D37" s="2">
+        <f t="shared" si="0"/>
+        <v>4035</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" ht="72" x14ac:dyDescent="0.3">
       <c r="A38" s="2" t="s">
         <v>74</v>
       </c>
       <c r="C38" s="3" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D38" s="2">
+        <f t="shared" si="0"/>
+        <v>4036</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>76</v>
       </c>
       <c r="C39" s="2" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D39" s="2">
+        <f t="shared" si="0"/>
+        <v>4037</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A40" s="4" t="s">
         <v>12</v>
       </c>
       <c r="C40" s="2" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="41" spans="1:3" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="D40" s="2">
+        <f t="shared" si="0"/>
+        <v>4038</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A41" s="4" t="s">
         <v>79</v>
       </c>
       <c r="C41" s="3" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="42" spans="1:3" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="D41" s="2">
+        <f t="shared" si="0"/>
+        <v>4039</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A42" s="4" t="s">
         <v>81</v>
       </c>
       <c r="C42" s="3" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D42" s="2">
+        <f t="shared" si="0"/>
+        <v>4040</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>83</v>
       </c>
       <c r="C43" s="2" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D43" s="2">
+        <f t="shared" si="0"/>
+        <v>4041</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A44" s="2" t="s">
         <v>85</v>
       </c>
       <c r="C44" s="2" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D44" s="2">
+        <f t="shared" si="0"/>
+        <v>4042</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A45" s="2" t="s">
         <v>87</v>
       </c>
       <c r="C45" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D45" s="2">
+        <f t="shared" si="0"/>
+        <v>4043</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A46" s="2" t="s">
         <v>89</v>
       </c>
       <c r="C46" s="2" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D46" s="2">
+        <f t="shared" si="0"/>
+        <v>4044</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A47" s="2" t="s">
         <v>91</v>
       </c>
       <c r="C47" s="2" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="48" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="D47" s="2">
+        <f t="shared" si="0"/>
+        <v>4045</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A48" s="2" t="s">
         <v>93</v>
       </c>
       <c r="C48" s="3" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D48" s="2">
+        <f t="shared" si="0"/>
+        <v>4046</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A49" s="2" t="s">
         <v>95</v>
       </c>
       <c r="C49" s="2" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="50" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="D49" s="2">
+        <f t="shared" si="0"/>
+        <v>4047</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A50" s="2" t="s">
         <v>97</v>
       </c>
       <c r="C50" s="3" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D50" s="2">
+        <f t="shared" si="0"/>
+        <v>4048</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A51" s="2" t="s">
         <v>99</v>
       </c>
       <c r="C51" s="2" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="52" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="D51" s="2">
+        <f t="shared" si="0"/>
+        <v>4049</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A52" s="2" t="s">
         <v>101</v>
       </c>
       <c r="C52" s="3" t="s">
         <v>102</v>
       </c>
-    </row>
-    <row r="53" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="D52" s="2">
+        <f t="shared" si="0"/>
+        <v>4050</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A53" s="2" t="s">
         <v>103</v>
       </c>
       <c r="C53" s="3" t="s">
         <v>104</v>
       </c>
-    </row>
-    <row r="54" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="D53" s="2">
+        <f t="shared" si="0"/>
+        <v>4051</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A54" s="2" t="s">
         <v>105</v>
       </c>
       <c r="C54" s="3" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D54" s="2">
+        <f t="shared" si="0"/>
+        <v>4052</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A55" s="2" t="s">
         <v>107</v>
       </c>
       <c r="C55" s="2" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D55" s="2">
+        <f t="shared" si="0"/>
+        <v>4053</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A56" s="2" t="s">
         <v>109</v>
       </c>
       <c r="C56" s="2" t="s">
         <v>110</v>
       </c>
-    </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D56" s="2">
+        <f t="shared" si="0"/>
+        <v>4054</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A57" s="2" t="s">
         <v>111</v>
       </c>
       <c r="C57" s="2" t="s">
         <v>112</v>
       </c>
-    </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D57" s="2">
+        <f t="shared" si="0"/>
+        <v>4055</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>113</v>
       </c>
       <c r="C58" s="2" t="s">
         <v>112</v>
       </c>
-    </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D58" s="2">
+        <f t="shared" si="0"/>
+        <v>4056</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A59" s="2" t="s">
         <v>114</v>
       </c>
       <c r="C59" s="2" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="60" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="D59" s="2">
+        <f t="shared" si="0"/>
+        <v>4057</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A60" s="2" t="s">
         <v>116</v>
       </c>
       <c r="C60" s="3" t="s">
         <v>117</v>
       </c>
-    </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D60" s="2">
+        <f t="shared" si="0"/>
+        <v>4058</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>118</v>
       </c>
       <c r="C61" s="2" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D61" s="2">
+        <f t="shared" si="0"/>
+        <v>4059</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A62" s="2" t="s">
         <v>120</v>
       </c>
       <c r="C62" t="s">
         <v>121</v>
       </c>
-    </row>
-    <row r="63" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="D62" s="2">
+        <f t="shared" si="0"/>
+        <v>4060</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A63" s="2" t="s">
         <v>122</v>
       </c>
       <c r="C63" s="3" t="s">
         <v>123</v>
       </c>
-    </row>
-    <row r="64" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="D63" s="2">
+        <f t="shared" si="0"/>
+        <v>4061</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A64" s="2" t="s">
         <v>124</v>
       </c>
       <c r="C64" s="3" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="65" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="D64" s="2">
+        <f t="shared" si="0"/>
+        <v>4062</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A65" s="2" t="s">
         <v>126</v>
       </c>
       <c r="C65" s="3" t="s">
         <v>127</v>
       </c>
-    </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D65" s="2">
+        <f t="shared" si="0"/>
+        <v>4063</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A66" s="2" t="s">
         <v>128</v>
       </c>
       <c r="C66" s="2" t="s">
         <v>129</v>
       </c>
-    </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D66" s="2">
+        <f t="shared" si="0"/>
+        <v>4064</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A67" s="2" t="s">
         <v>130</v>
       </c>
       <c r="C67" s="2" t="s">
         <v>131</v>
       </c>
-    </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D67" s="2">
+        <f t="shared" si="0"/>
+        <v>4065</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A68" s="2" t="s">
         <v>132</v>
       </c>
       <c r="C68" s="2" t="s">
         <v>133</v>
       </c>
-    </row>
-    <row r="69" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="D68" s="2">
+        <f t="shared" ref="D68:D131" si="1">D67+1</f>
+        <v>4066</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A69" s="2" t="s">
         <v>134</v>
       </c>
       <c r="C69" s="3" t="s">
         <v>135</v>
       </c>
-    </row>
-    <row r="70" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="D69" s="2">
+        <f t="shared" si="1"/>
+        <v>4067</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A70" s="2" t="s">
         <v>136</v>
       </c>
       <c r="C70" s="3" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="71" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="D70" s="2">
+        <f t="shared" si="1"/>
+        <v>4068</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A71" s="2" t="s">
         <v>138</v>
       </c>
       <c r="C71" s="3" t="s">
         <v>139</v>
       </c>
-    </row>
-    <row r="72" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="D71" s="2">
+        <f t="shared" si="1"/>
+        <v>4069</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A72" s="3" t="s">
         <v>140</v>
       </c>
       <c r="C72" s="3" t="s">
         <v>141</v>
       </c>
-    </row>
-    <row r="73" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="D72" s="2">
+        <f t="shared" si="1"/>
+        <v>4070</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A73" s="2" t="s">
         <v>142</v>
       </c>
       <c r="C73" s="3" t="s">
         <v>143</v>
       </c>
-    </row>
-    <row r="74" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="D73" s="2">
+        <f t="shared" si="1"/>
+        <v>4071</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A74" s="2" t="s">
         <v>144</v>
       </c>
       <c r="C74" s="3" t="s">
         <v>145</v>
       </c>
-    </row>
-    <row r="75" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="D74" s="2">
+        <f t="shared" si="1"/>
+        <v>4072</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A75" s="2" t="s">
         <v>146</v>
       </c>
       <c r="C75" s="3" t="s">
         <v>147</v>
       </c>
-    </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D75" s="2">
+        <f t="shared" si="1"/>
+        <v>4073</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A76" s="2" t="s">
         <v>148</v>
       </c>
       <c r="C76" s="2" t="s">
         <v>149</v>
       </c>
-    </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D76" s="2">
+        <f t="shared" si="1"/>
+        <v>4074</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A77" s="2" t="s">
         <v>150</v>
       </c>
       <c r="C77" s="2" t="s">
         <v>151</v>
       </c>
-    </row>
-    <row r="78" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="D77" s="2">
+        <f t="shared" si="1"/>
+        <v>4075</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A78" s="2" t="s">
         <v>152</v>
       </c>
       <c r="C78" s="3" t="s">
         <v>153</v>
       </c>
-    </row>
-    <row r="79" spans="1:3" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="D78" s="2">
+        <f t="shared" si="1"/>
+        <v>4076</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A79" s="2" t="s">
         <v>154</v>
       </c>
       <c r="C79" s="3" t="s">
         <v>155</v>
       </c>
-    </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D79" s="2">
+        <f t="shared" si="1"/>
+        <v>4077</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A80" s="2" t="s">
         <v>156</v>
       </c>
       <c r="C80" s="2" t="s">
         <v>157</v>
       </c>
-    </row>
-    <row r="81" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="D80" s="2">
+        <f t="shared" si="1"/>
+        <v>4078</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A81" s="2" t="s">
         <v>158</v>
       </c>
       <c r="C81" s="3" t="s">
         <v>159</v>
       </c>
-    </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D81" s="2">
+        <f t="shared" si="1"/>
+        <v>4079</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A82" s="2" t="s">
         <v>160</v>
       </c>
       <c r="C82" s="2" t="s">
         <v>161</v>
       </c>
-    </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D82" s="2">
+        <f t="shared" si="1"/>
+        <v>4080</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A83" s="2" t="s">
         <v>162</v>
       </c>
       <c r="C83" s="2" t="s">
         <v>163</v>
       </c>
-    </row>
-    <row r="84" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="D83" s="2">
+        <f t="shared" si="1"/>
+        <v>4081</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A84" s="2" t="s">
         <v>164</v>
       </c>
       <c r="C84" s="3" t="s">
         <v>165</v>
       </c>
-    </row>
-    <row r="85" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="D84" s="2">
+        <f t="shared" si="1"/>
+        <v>4082</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A85" s="2" t="s">
         <v>166</v>
       </c>
       <c r="C85" s="3" t="s">
         <v>167</v>
       </c>
-    </row>
-    <row r="86" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="D85" s="2">
+        <f t="shared" si="1"/>
+        <v>4083</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A86" s="2" t="s">
         <v>168</v>
       </c>
       <c r="C86" s="3" t="s">
         <v>169</v>
       </c>
-    </row>
-    <row r="87" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="D86" s="2">
+        <f t="shared" si="1"/>
+        <v>4084</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A87" s="2" t="s">
         <v>170</v>
       </c>
       <c r="C87" s="3" t="s">
         <v>171</v>
       </c>
-    </row>
-    <row r="88" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="D87" s="2">
+        <f t="shared" si="1"/>
+        <v>4085</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A88" s="2" t="s">
         <v>172</v>
       </c>
       <c r="C88" s="3" t="s">
         <v>173</v>
       </c>
-    </row>
-    <row r="89" spans="1:3" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="D88" s="2">
+        <f t="shared" si="1"/>
+        <v>4086</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A89" s="2" t="s">
         <v>174</v>
       </c>
       <c r="C89" s="3" t="s">
         <v>175</v>
       </c>
-    </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D89" s="2">
+        <f t="shared" si="1"/>
+        <v>4087</v>
+      </c>
+    </row>
+    <row r="90" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A90" s="2" t="s">
         <v>176</v>
       </c>
       <c r="C90" s="2" t="s">
         <v>177</v>
       </c>
-    </row>
-    <row r="91" spans="1:3" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="D90" s="2">
+        <f t="shared" si="1"/>
+        <v>4088</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A91" s="2" t="s">
         <v>178</v>
       </c>
       <c r="C91" s="3" t="s">
         <v>179</v>
       </c>
-    </row>
-    <row r="92" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="D91" s="2">
+        <f t="shared" si="1"/>
+        <v>4089</v>
+      </c>
+    </row>
+    <row r="92" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A92" s="2" t="s">
         <v>180</v>
       </c>
       <c r="C92" s="3" t="s">
         <v>181</v>
       </c>
-    </row>
-    <row r="93" spans="1:3" ht="115.2" x14ac:dyDescent="0.3">
+      <c r="D92" s="2">
+        <f t="shared" si="1"/>
+        <v>4090</v>
+      </c>
+    </row>
+    <row r="93" spans="1:4" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A93" s="2" t="s">
         <v>182</v>
       </c>
       <c r="C93" s="3" t="s">
         <v>183</v>
       </c>
-    </row>
-    <row r="94" spans="1:3" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="D93" s="2">
+        <f t="shared" si="1"/>
+        <v>4091</v>
+      </c>
+    </row>
+    <row r="94" spans="1:4" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A94" s="2" t="s">
         <v>184</v>
       </c>
       <c r="C94" s="3" t="s">
         <v>185</v>
       </c>
-    </row>
-    <row r="95" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D94" s="2">
+        <f t="shared" si="1"/>
+        <v>4092</v>
+      </c>
+    </row>
+    <row r="95" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A95" s="2" t="s">
         <v>186</v>
       </c>
       <c r="C95" s="2" t="s">
         <v>187</v>
       </c>
-    </row>
-    <row r="96" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="D95" s="2">
+        <f t="shared" si="1"/>
+        <v>4093</v>
+      </c>
+    </row>
+    <row r="96" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A96" s="2" t="s">
         <v>188</v>
       </c>
       <c r="C96" s="3" t="s">
         <v>189</v>
       </c>
-    </row>
-    <row r="97" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="D96" s="2">
+        <f t="shared" si="1"/>
+        <v>4094</v>
+      </c>
+    </row>
+    <row r="97" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A97" s="2" t="s">
         <v>190</v>
       </c>
       <c r="C97" s="3" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="98" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D97" s="2">
+        <f t="shared" si="1"/>
+        <v>4095</v>
+      </c>
+    </row>
+    <row r="98" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A98" s="2" t="s">
         <v>192</v>
       </c>
       <c r="C98" s="2" t="s">
         <v>193</v>
       </c>
-    </row>
-    <row r="99" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="D98" s="2">
+        <f t="shared" si="1"/>
+        <v>4096</v>
+      </c>
+    </row>
+    <row r="99" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A99" s="2" t="s">
         <v>194</v>
       </c>
       <c r="C99" s="3" t="s">
         <v>195</v>
       </c>
-    </row>
-    <row r="100" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D99" s="2">
+        <f t="shared" si="1"/>
+        <v>4097</v>
+      </c>
+    </row>
+    <row r="100" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A100" s="2" t="s">
         <v>196</v>
       </c>
       <c r="C100" s="2" t="s">
         <v>197</v>
       </c>
-    </row>
-    <row r="101" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="D100" s="2">
+        <f t="shared" si="1"/>
+        <v>4098</v>
+      </c>
+    </row>
+    <row r="101" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A101" s="2" t="s">
         <v>198</v>
       </c>
       <c r="C101" s="3" t="s">
         <v>199</v>
       </c>
-    </row>
-    <row r="102" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D101" s="2">
+        <f t="shared" si="1"/>
+        <v>4099</v>
+      </c>
+    </row>
+    <row r="102" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A102" s="2" t="s">
         <v>200</v>
       </c>
       <c r="C102" s="2" t="s">
         <v>201</v>
       </c>
-    </row>
-    <row r="103" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D102" s="2">
+        <f t="shared" si="1"/>
+        <v>4100</v>
+      </c>
+    </row>
+    <row r="103" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A103" s="2" t="s">
         <v>202</v>
       </c>
       <c r="C103" s="2" t="s">
         <v>203</v>
       </c>
-    </row>
-    <row r="104" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D103" s="2">
+        <f t="shared" si="1"/>
+        <v>4101</v>
+      </c>
+    </row>
+    <row r="104" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A104" s="2" t="s">
         <v>204</v>
       </c>
       <c r="C104" s="2" t="s">
         <v>205</v>
       </c>
-    </row>
-    <row r="105" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D104" s="2">
+        <f t="shared" si="1"/>
+        <v>4102</v>
+      </c>
+    </row>
+    <row r="105" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A105" s="2" t="s">
         <v>206</v>
       </c>
       <c r="C105" s="2" t="s">
         <v>207</v>
       </c>
-    </row>
-    <row r="106" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="D105" s="2">
+        <f t="shared" si="1"/>
+        <v>4103</v>
+      </c>
+    </row>
+    <row r="106" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A106" s="2" t="s">
         <v>208</v>
       </c>
       <c r="C106" s="3" t="s">
         <v>209</v>
       </c>
-    </row>
-    <row r="107" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D106" s="2">
+        <f t="shared" si="1"/>
+        <v>4104</v>
+      </c>
+    </row>
+    <row r="107" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A107" s="2" t="s">
         <v>210</v>
       </c>
       <c r="C107" s="2" t="s">
         <v>211</v>
       </c>
-    </row>
-    <row r="108" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D107" s="2">
+        <f t="shared" si="1"/>
+        <v>4105</v>
+      </c>
+    </row>
+    <row r="108" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A108" s="2" t="s">
         <v>212</v>
       </c>
       <c r="C108" s="2" t="s">
         <v>213</v>
       </c>
-    </row>
-    <row r="109" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D108" s="2">
+        <f t="shared" si="1"/>
+        <v>4106</v>
+      </c>
+    </row>
+    <row r="109" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A109" s="2" t="s">
         <v>214</v>
       </c>
       <c r="C109" s="2" t="s">
         <v>215</v>
       </c>
-    </row>
-    <row r="110" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="D109" s="2">
+        <f t="shared" si="1"/>
+        <v>4107</v>
+      </c>
+    </row>
+    <row r="110" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A110" s="2" t="s">
         <v>216</v>
       </c>
       <c r="C110" s="3" t="s">
         <v>217</v>
       </c>
-    </row>
-    <row r="111" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="D110" s="2">
+        <f t="shared" si="1"/>
+        <v>4108</v>
+      </c>
+    </row>
+    <row r="111" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A111" s="2" t="s">
         <v>218</v>
       </c>
       <c r="C111" s="3" t="s">
         <v>219</v>
       </c>
-    </row>
-    <row r="112" spans="1:3" ht="158.4" x14ac:dyDescent="0.3">
+      <c r="D111" s="2">
+        <f t="shared" si="1"/>
+        <v>4109</v>
+      </c>
+    </row>
+    <row r="112" spans="1:4" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A112" s="2" t="s">
         <v>220</v>
       </c>
       <c r="C112" s="3" t="s">
         <v>221</v>
       </c>
-    </row>
-    <row r="113" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="D112" s="2">
+        <f t="shared" si="1"/>
+        <v>4110</v>
+      </c>
+    </row>
+    <row r="113" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A113" s="2" t="s">
         <v>222</v>
       </c>
       <c r="C113" s="3" t="s">
         <v>223</v>
       </c>
-    </row>
-    <row r="114" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D113" s="2">
+        <f t="shared" si="1"/>
+        <v>4111</v>
+      </c>
+    </row>
+    <row r="114" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A114" s="2" t="s">
         <v>224</v>
       </c>
       <c r="C114" s="2" t="s">
         <v>225</v>
       </c>
-    </row>
-    <row r="115" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="D114" s="2">
+        <f t="shared" si="1"/>
+        <v>4112</v>
+      </c>
+    </row>
+    <row r="115" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A115" s="2" t="s">
         <v>226</v>
       </c>
       <c r="C115" s="3" t="s">
         <v>227</v>
       </c>
-    </row>
-    <row r="116" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="D115" s="2">
+        <f t="shared" si="1"/>
+        <v>4113</v>
+      </c>
+    </row>
+    <row r="116" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A116" s="2" t="s">
         <v>228</v>
       </c>
       <c r="C116" s="3" t="s">
         <v>229</v>
       </c>
-    </row>
-    <row r="117" spans="1:3" ht="72" x14ac:dyDescent="0.3">
+      <c r="D116" s="2">
+        <f t="shared" si="1"/>
+        <v>4114</v>
+      </c>
+    </row>
+    <row r="117" spans="1:4" ht="72" x14ac:dyDescent="0.3">
       <c r="A117" s="2" t="s">
         <v>230</v>
       </c>
       <c r="C117" s="3" t="s">
         <v>231</v>
       </c>
-    </row>
-    <row r="118" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="D117" s="2">
+        <f t="shared" si="1"/>
+        <v>4115</v>
+      </c>
+    </row>
+    <row r="118" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A118" s="3" t="s">
         <v>232</v>
       </c>
       <c r="C118" s="3" t="s">
         <v>233</v>
       </c>
-    </row>
-    <row r="119" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="D118" s="2">
+        <f t="shared" si="1"/>
+        <v>4116</v>
+      </c>
+    </row>
+    <row r="119" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A119" s="3" t="s">
         <v>234</v>
       </c>
       <c r="C119" s="3" t="s">
         <v>235</v>
       </c>
-    </row>
-    <row r="120" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="D119" s="2">
+        <f t="shared" si="1"/>
+        <v>4117</v>
+      </c>
+    </row>
+    <row r="120" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A120" s="2" t="s">
         <v>236</v>
       </c>
       <c r="C120" s="3" t="s">
         <v>237</v>
       </c>
-    </row>
-    <row r="121" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="D120" s="2">
+        <f t="shared" si="1"/>
+        <v>4118</v>
+      </c>
+    </row>
+    <row r="121" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A121" s="2" t="s">
         <v>238</v>
       </c>
       <c r="C121" s="3" t="s">
         <v>239</v>
       </c>
-    </row>
-    <row r="122" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="D121" s="2">
+        <f t="shared" si="1"/>
+        <v>4119</v>
+      </c>
+    </row>
+    <row r="122" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A122" s="2" t="s">
         <v>240</v>
       </c>
       <c r="C122" s="3" t="s">
         <v>241</v>
       </c>
-    </row>
-    <row r="123" spans="1:3" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="D122" s="2">
+        <f t="shared" si="1"/>
+        <v>4120</v>
+      </c>
+    </row>
+    <row r="123" spans="1:4" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A123" s="2" t="s">
         <v>242</v>
       </c>
       <c r="C123" s="3" t="s">
         <v>243</v>
       </c>
-    </row>
-    <row r="124" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D123" s="2">
+        <f t="shared" si="1"/>
+        <v>4121</v>
+      </c>
+    </row>
+    <row r="124" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A124" s="2" t="s">
         <v>244</v>
       </c>
       <c r="C124" s="2" t="s">
         <v>245</v>
       </c>
-    </row>
-    <row r="125" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="D124" s="2">
+        <f t="shared" si="1"/>
+        <v>4122</v>
+      </c>
+    </row>
+    <row r="125" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A125" s="3" t="s">
         <v>246</v>
       </c>
       <c r="C125" s="3" t="s">
         <v>247</v>
       </c>
-    </row>
-    <row r="126" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="D125" s="2">
+        <f t="shared" si="1"/>
+        <v>4123</v>
+      </c>
+    </row>
+    <row r="126" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A126" s="2" t="s">
         <v>248</v>
       </c>
       <c r="C126" s="3" t="s">
         <v>249</v>
       </c>
-    </row>
-    <row r="127" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="D126" s="2">
+        <f t="shared" si="1"/>
+        <v>4124</v>
+      </c>
+    </row>
+    <row r="127" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A127" s="2" t="s">
         <v>250</v>
       </c>
       <c r="C127" s="3" t="s">
         <v>251</v>
       </c>
-    </row>
-    <row r="128" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D127" s="2">
+        <f t="shared" si="1"/>
+        <v>4125</v>
+      </c>
+    </row>
+    <row r="128" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A128" s="2" t="s">
         <v>252</v>
       </c>
       <c r="C128" s="2" t="s">
         <v>253</v>
       </c>
-    </row>
-    <row r="129" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D128" s="2">
+        <f t="shared" si="1"/>
+        <v>4126</v>
+      </c>
+    </row>
+    <row r="129" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A129" s="2" t="s">
         <v>254</v>
       </c>
       <c r="C129" s="2" t="s">
         <v>255</v>
       </c>
-    </row>
-    <row r="130" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D129" s="2">
+        <f t="shared" si="1"/>
+        <v>4127</v>
+      </c>
+    </row>
+    <row r="130" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A130" s="2" t="s">
         <v>256</v>
       </c>
       <c r="C130" s="2" t="s">
         <v>257</v>
       </c>
-    </row>
-    <row r="131" spans="1:3" ht="115.2" x14ac:dyDescent="0.3">
+      <c r="D130" s="2">
+        <f t="shared" si="1"/>
+        <v>4128</v>
+      </c>
+    </row>
+    <row r="131" spans="1:4" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A131" s="2" t="s">
         <v>258</v>
       </c>
       <c r="C131" s="3" t="s">
         <v>259</v>
       </c>
-    </row>
-    <row r="132" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="D131" s="2">
+        <f t="shared" si="1"/>
+        <v>4129</v>
+      </c>
+    </row>
+    <row r="132" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A132" s="2" t="s">
         <v>260</v>
       </c>
       <c r="C132" s="3" t="s">
         <v>261</v>
       </c>
-    </row>
-    <row r="133" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="D132" s="2">
+        <f t="shared" ref="D132:D177" si="2">D131+1</f>
+        <v>4130</v>
+      </c>
+    </row>
+    <row r="133" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A133" s="2" t="s">
         <v>262</v>
       </c>
       <c r="C133" s="3" t="s">
         <v>263</v>
       </c>
-    </row>
-    <row r="134" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="D133" s="2">
+        <f t="shared" si="2"/>
+        <v>4131</v>
+      </c>
+    </row>
+    <row r="134" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A134" s="2" t="s">
         <v>264</v>
       </c>
       <c r="C134" s="3" t="s">
         <v>265</v>
       </c>
-    </row>
-    <row r="135" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D134" s="2">
+        <f t="shared" si="2"/>
+        <v>4132</v>
+      </c>
+    </row>
+    <row r="135" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A135" s="2" t="s">
         <v>266</v>
       </c>
       <c r="C135" s="2" t="s">
         <v>267</v>
       </c>
-    </row>
-    <row r="136" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="D135" s="2">
+        <f t="shared" si="2"/>
+        <v>4133</v>
+      </c>
+    </row>
+    <row r="136" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A136" s="2" t="s">
         <v>268</v>
       </c>
       <c r="C136" s="3" t="s">
         <v>269</v>
       </c>
-    </row>
-    <row r="137" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D136" s="2">
+        <f t="shared" si="2"/>
+        <v>4134</v>
+      </c>
+    </row>
+    <row r="137" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A137" s="2" t="s">
         <v>270</v>
       </c>
       <c r="C137" s="2" t="s">
         <v>271</v>
       </c>
-    </row>
-    <row r="138" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="D137" s="2">
+        <f t="shared" si="2"/>
+        <v>4135</v>
+      </c>
+    </row>
+    <row r="138" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A138" s="2" t="s">
         <v>272</v>
       </c>
       <c r="C138" s="3" t="s">
         <v>273</v>
       </c>
-    </row>
-    <row r="139" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D138" s="2">
+        <f t="shared" si="2"/>
+        <v>4136</v>
+      </c>
+    </row>
+    <row r="139" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A139" s="2" t="s">
         <v>274</v>
       </c>
       <c r="C139" s="2" t="s">
         <v>275</v>
       </c>
-    </row>
-    <row r="140" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D139" s="2">
+        <f t="shared" si="2"/>
+        <v>4137</v>
+      </c>
+    </row>
+    <row r="140" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A140" s="2" t="s">
         <v>276</v>
       </c>
       <c r="C140" s="2" t="s">
         <v>277</v>
       </c>
-    </row>
-    <row r="141" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="D140" s="2">
+        <f t="shared" si="2"/>
+        <v>4138</v>
+      </c>
+    </row>
+    <row r="141" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A141" s="2" t="s">
         <v>278</v>
       </c>
       <c r="C141" s="3" t="s">
         <v>279</v>
       </c>
-    </row>
-    <row r="142" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D141" s="2">
+        <f t="shared" si="2"/>
+        <v>4139</v>
+      </c>
+    </row>
+    <row r="142" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A142" s="2" t="s">
         <v>280</v>
       </c>
       <c r="C142" s="2" t="s">
         <v>281</v>
       </c>
-    </row>
-    <row r="143" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="D142" s="2">
+        <f t="shared" si="2"/>
+        <v>4140</v>
+      </c>
+    </row>
+    <row r="143" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A143" s="3" t="s">
         <v>282</v>
       </c>
       <c r="C143" s="3" t="s">
         <v>283</v>
       </c>
-    </row>
-    <row r="144" spans="1:3" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="D143" s="2">
+        <f t="shared" si="2"/>
+        <v>4141</v>
+      </c>
+    </row>
+    <row r="144" spans="1:4" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A144" s="3" t="s">
         <v>284</v>
       </c>
       <c r="C144" s="3" t="s">
         <v>285</v>
       </c>
-    </row>
-    <row r="145" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D144" s="2">
+        <f t="shared" si="2"/>
+        <v>4142</v>
+      </c>
+    </row>
+    <row r="145" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A145" s="2" t="s">
         <v>286</v>
       </c>
       <c r="C145" s="2" t="s">
         <v>287</v>
       </c>
-    </row>
-    <row r="146" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="D145" s="2">
+        <f t="shared" si="2"/>
+        <v>4143</v>
+      </c>
+    </row>
+    <row r="146" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A146" s="2" t="s">
         <v>288</v>
       </c>
       <c r="C146" s="3" t="s">
         <v>289</v>
       </c>
-    </row>
-    <row r="147" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="D146" s="2">
+        <f t="shared" si="2"/>
+        <v>4144</v>
+      </c>
+    </row>
+    <row r="147" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A147" s="2" t="s">
         <v>290</v>
       </c>
       <c r="C147" s="3" t="s">
         <v>291</v>
       </c>
-    </row>
-    <row r="148" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="D147" s="2">
+        <f t="shared" si="2"/>
+        <v>4145</v>
+      </c>
+    </row>
+    <row r="148" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A148" s="2" t="s">
         <v>292</v>
       </c>
       <c r="C148" s="3" t="s">
         <v>293</v>
       </c>
-    </row>
-    <row r="149" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="D148" s="2">
+        <f t="shared" si="2"/>
+        <v>4146</v>
+      </c>
+    </row>
+    <row r="149" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A149" s="2" t="s">
         <v>294</v>
       </c>
       <c r="C149" s="3" t="s">
         <v>295</v>
       </c>
-    </row>
-    <row r="150" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D149" s="2">
+        <f t="shared" si="2"/>
+        <v>4147</v>
+      </c>
+    </row>
+    <row r="150" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A150" s="2" t="s">
         <v>296</v>
       </c>
       <c r="C150" s="2" t="s">
         <v>297</v>
       </c>
-    </row>
-    <row r="151" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D150" s="2">
+        <f t="shared" si="2"/>
+        <v>4148</v>
+      </c>
+    </row>
+    <row r="151" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A151" s="2" t="s">
         <v>298</v>
       </c>
       <c r="C151" s="2" t="s">
         <v>299</v>
       </c>
-    </row>
-    <row r="152" spans="1:3" ht="129.6" x14ac:dyDescent="0.3">
+      <c r="D151" s="2">
+        <f t="shared" si="2"/>
+        <v>4149</v>
+      </c>
+    </row>
+    <row r="152" spans="1:4" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A152" s="2" t="s">
         <v>300</v>
       </c>
       <c r="C152" s="3" t="s">
         <v>301</v>
       </c>
-    </row>
-    <row r="153" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="D152" s="2">
+        <f t="shared" si="2"/>
+        <v>4150</v>
+      </c>
+    </row>
+    <row r="153" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A153" s="2" t="s">
         <v>302</v>
       </c>
       <c r="C153" s="3" t="s">
         <v>303</v>
       </c>
-    </row>
-    <row r="154" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="D153" s="2">
+        <f t="shared" si="2"/>
+        <v>4151</v>
+      </c>
+    </row>
+    <row r="154" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A154" s="2" t="s">
         <v>304</v>
       </c>
       <c r="C154" s="3" t="s">
         <v>305</v>
       </c>
-    </row>
-    <row r="155" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D154" s="2">
+        <f t="shared" si="2"/>
+        <v>4152</v>
+      </c>
+    </row>
+    <row r="155" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A155" s="2" t="s">
         <v>306</v>
       </c>
       <c r="C155" s="2" t="s">
         <v>307</v>
       </c>
-    </row>
-    <row r="156" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="D155" s="2">
+        <f t="shared" si="2"/>
+        <v>4153</v>
+      </c>
+    </row>
+    <row r="156" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A156" s="2" t="s">
         <v>308</v>
       </c>
       <c r="C156" s="3" t="s">
         <v>309</v>
       </c>
-    </row>
-    <row r="157" spans="1:3" ht="115.2" x14ac:dyDescent="0.3">
+      <c r="D156" s="2">
+        <f t="shared" si="2"/>
+        <v>4154</v>
+      </c>
+    </row>
+    <row r="157" spans="1:4" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A157" s="2" t="s">
         <v>310</v>
       </c>
       <c r="C157" s="3" t="s">
         <v>311</v>
       </c>
-    </row>
-    <row r="158" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="D157" s="2">
+        <f t="shared" si="2"/>
+        <v>4155</v>
+      </c>
+    </row>
+    <row r="158" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A158" s="2" t="s">
         <v>312</v>
       </c>
       <c r="C158" s="3" t="s">
         <v>313</v>
       </c>
-    </row>
-    <row r="159" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="D158" s="2">
+        <f t="shared" si="2"/>
+        <v>4156</v>
+      </c>
+    </row>
+    <row r="159" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A159" s="2" t="s">
         <v>314</v>
       </c>
       <c r="C159" s="3" t="s">
         <v>315</v>
       </c>
-    </row>
-    <row r="160" spans="1:3" ht="72" x14ac:dyDescent="0.3">
+      <c r="D159" s="2">
+        <f t="shared" si="2"/>
+        <v>4157</v>
+      </c>
+    </row>
+    <row r="160" spans="1:4" ht="72" x14ac:dyDescent="0.3">
       <c r="A160" s="2" t="s">
         <v>316</v>
       </c>
       <c r="C160" s="3" t="s">
         <v>317</v>
       </c>
-    </row>
-    <row r="161" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="D160" s="2">
+        <f t="shared" si="2"/>
+        <v>4158</v>
+      </c>
+    </row>
+    <row r="161" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A161" s="2" t="s">
         <v>318</v>
       </c>
       <c r="C161" s="3" t="s">
         <v>319</v>
       </c>
-    </row>
-    <row r="162" spans="1:3" ht="72" x14ac:dyDescent="0.3">
+      <c r="D161" s="2">
+        <f t="shared" si="2"/>
+        <v>4159</v>
+      </c>
+    </row>
+    <row r="162" spans="1:4" ht="72" x14ac:dyDescent="0.3">
       <c r="A162" s="2" t="s">
         <v>320</v>
       </c>
       <c r="C162" s="3" t="s">
         <v>321</v>
       </c>
-    </row>
-    <row r="163" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="D162" s="2">
+        <f t="shared" si="2"/>
+        <v>4160</v>
+      </c>
+    </row>
+    <row r="163" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A163" s="2" t="s">
         <v>322</v>
       </c>
       <c r="C163" s="3" t="s">
         <v>323</v>
       </c>
-    </row>
-    <row r="164" spans="1:3" ht="187.2" x14ac:dyDescent="0.3">
+      <c r="D163" s="2">
+        <f t="shared" si="2"/>
+        <v>4161</v>
+      </c>
+    </row>
+    <row r="164" spans="1:4" ht="187.2" x14ac:dyDescent="0.3">
       <c r="A164" s="2" t="s">
         <v>324</v>
       </c>
       <c r="C164" s="3" t="s">
         <v>325</v>
       </c>
-    </row>
-    <row r="165" spans="1:3" ht="144" x14ac:dyDescent="0.3">
+      <c r="D164" s="2">
+        <f t="shared" si="2"/>
+        <v>4162</v>
+      </c>
+    </row>
+    <row r="165" spans="1:4" ht="144" x14ac:dyDescent="0.3">
       <c r="A165" s="2" t="s">
         <v>326</v>
       </c>
       <c r="C165" s="3" t="s">
         <v>327</v>
       </c>
-    </row>
-    <row r="166" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D165" s="2">
+        <f t="shared" si="2"/>
+        <v>4163</v>
+      </c>
+    </row>
+    <row r="166" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A166" s="2" t="s">
         <v>328</v>
       </c>
       <c r="C166" s="2" t="s">
         <v>329</v>
       </c>
-    </row>
-    <row r="167" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="D166" s="2">
+        <f t="shared" si="2"/>
+        <v>4164</v>
+      </c>
+    </row>
+    <row r="167" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A167" s="2" t="s">
         <v>330</v>
       </c>
       <c r="C167" s="3" t="s">
         <v>331</v>
       </c>
-    </row>
-    <row r="168" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="D167" s="2">
+        <f t="shared" si="2"/>
+        <v>4165</v>
+      </c>
+    </row>
+    <row r="168" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A168" s="2" t="s">
         <v>332</v>
       </c>
       <c r="C168" s="3" t="s">
         <v>333</v>
       </c>
-    </row>
-    <row r="169" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D168" s="2">
+        <f t="shared" si="2"/>
+        <v>4166</v>
+      </c>
+    </row>
+    <row r="169" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A169" s="2" t="s">
         <v>334</v>
       </c>
       <c r="C169" s="2" t="s">
         <v>335</v>
       </c>
-    </row>
-    <row r="170" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="D169" s="2">
+        <f t="shared" si="2"/>
+        <v>4167</v>
+      </c>
+    </row>
+    <row r="170" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A170" s="2" t="s">
         <v>336</v>
       </c>
       <c r="C170" s="3" t="s">
         <v>337</v>
       </c>
-    </row>
-    <row r="171" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D170" s="2">
+        <f t="shared" si="2"/>
+        <v>4168</v>
+      </c>
+    </row>
+    <row r="171" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A171" s="2" t="s">
         <v>338</v>
       </c>
       <c r="C171" s="2" t="s">
         <v>339</v>
       </c>
-    </row>
-    <row r="172" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="D171" s="2">
+        <f t="shared" si="2"/>
+        <v>4169</v>
+      </c>
+    </row>
+    <row r="172" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A172" s="2" t="s">
         <v>340</v>
       </c>
       <c r="C172" s="3" t="s">
         <v>341</v>
       </c>
-    </row>
-    <row r="173" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="D172" s="2">
+        <f t="shared" si="2"/>
+        <v>4170</v>
+      </c>
+    </row>
+    <row r="173" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A173" s="2" t="s">
         <v>342</v>
       </c>
       <c r="C173" s="3" t="s">
         <v>343</v>
       </c>
-    </row>
-    <row r="174" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="D173" s="2">
+        <f t="shared" si="2"/>
+        <v>4171</v>
+      </c>
+    </row>
+    <row r="174" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A174" s="2" t="s">
         <v>344</v>
       </c>
       <c r="C174" s="3" t="s">
         <v>345</v>
       </c>
-    </row>
-    <row r="175" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D174" s="2">
+        <f t="shared" si="2"/>
+        <v>4172</v>
+      </c>
+    </row>
+    <row r="175" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A175" s="2" t="s">
         <v>344</v>
       </c>
       <c r="C175" s="2" t="s">
         <v>346</v>
       </c>
-    </row>
-    <row r="176" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D175" s="2">
+        <f t="shared" si="2"/>
+        <v>4173</v>
+      </c>
+    </row>
+    <row r="176" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A176" s="2" t="s">
         <v>347</v>
       </c>
       <c r="C176" s="2" t="s">
         <v>348</v>
       </c>
-    </row>
-    <row r="177" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="D176" s="2">
+        <f t="shared" si="2"/>
+        <v>4174</v>
+      </c>
+    </row>
+    <row r="177" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A177" s="2" t="s">
         <v>349</v>
       </c>
       <c r="C177" s="3" t="s">
         <v>350</v>
+      </c>
+      <c r="D177" s="2">
+        <f t="shared" si="2"/>
+        <v>4175</v>
       </c>
     </row>
     <row r="298" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
@@ -3877,7 +4602,7 @@
         <v>1</v>
       </c>
       <c r="E1" s="6" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="50.4" x14ac:dyDescent="0.3">
@@ -4193,8 +4918,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C2F12F5D-B06A-4DED-8C5D-17DDBB4DFB56}">
   <dimension ref="A1:E31"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B29" sqref="B29"/>
+    <sheetView topLeftCell="A29" workbookViewId="0">
+      <selection activeCell="D33" sqref="D33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4217,6 +4942,9 @@
       <c r="D1" s="13" t="s">
         <v>1</v>
       </c>
+      <c r="E1" s="13" t="s">
+        <v>560</v>
+      </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
@@ -4228,6 +4956,9 @@
       <c r="D2" s="6" t="s">
         <v>473</v>
       </c>
+      <c r="E2">
+        <v>3000</v>
+      </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
@@ -4236,6 +4967,10 @@
       <c r="D3" s="6" t="s">
         <v>475</v>
       </c>
+      <c r="E3">
+        <f>E2+1</f>
+        <v>3001</v>
+      </c>
     </row>
     <row r="4" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
@@ -4244,6 +4979,10 @@
       <c r="D4" s="6" t="s">
         <v>477</v>
       </c>
+      <c r="E4">
+        <f t="shared" ref="E4:E31" si="0">E3+1</f>
+        <v>3002</v>
+      </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
@@ -4252,6 +4991,10 @@
       <c r="D5" s="6" t="s">
         <v>479</v>
       </c>
+      <c r="E5">
+        <f t="shared" si="0"/>
+        <v>3003</v>
+      </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
@@ -4263,6 +5006,10 @@
       <c r="D6" s="6" t="s">
         <v>482</v>
       </c>
+      <c r="E6">
+        <f t="shared" si="0"/>
+        <v>3004</v>
+      </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B7" t="s">
@@ -4271,6 +5018,10 @@
       <c r="D7" s="6" t="s">
         <v>484</v>
       </c>
+      <c r="E7">
+        <f t="shared" si="0"/>
+        <v>3005</v>
+      </c>
     </row>
     <row r="8" spans="1:5" ht="42" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B8" s="2" t="s">
@@ -4279,8 +5030,9 @@
       <c r="D8" s="3" t="s">
         <v>486</v>
       </c>
-      <c r="E8" t="s">
-        <v>482</v>
+      <c r="E8">
+        <f t="shared" si="0"/>
+        <v>3006</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
@@ -4290,8 +5042,9 @@
       <c r="D9" s="6" t="s">
         <v>488</v>
       </c>
-      <c r="E9" t="s">
-        <v>482</v>
+      <c r="E9">
+        <f t="shared" si="0"/>
+        <v>3007</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
@@ -4301,6 +5054,10 @@
       <c r="D10" s="6" t="s">
         <v>490</v>
       </c>
+      <c r="E10">
+        <f t="shared" si="0"/>
+        <v>3008</v>
+      </c>
     </row>
     <row r="11" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B11" t="s">
@@ -4309,8 +5066,9 @@
       <c r="D11" s="6" t="s">
         <v>492</v>
       </c>
-      <c r="E11" t="s">
-        <v>482</v>
+      <c r="E11">
+        <f t="shared" si="0"/>
+        <v>3009</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
@@ -4320,10 +5078,15 @@
       <c r="D12" s="6" t="s">
         <v>494</v>
       </c>
+      <c r="E12">
+        <f t="shared" si="0"/>
+        <v>3010</v>
+      </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="E13" t="s">
-        <v>482</v>
+      <c r="E13">
+        <f t="shared" si="0"/>
+        <v>3011</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.3">
@@ -4333,6 +5096,10 @@
       <c r="D14" s="6" t="s">
         <v>496</v>
       </c>
+      <c r="E14">
+        <f t="shared" si="0"/>
+        <v>3012</v>
+      </c>
     </row>
     <row r="15" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B15" t="s">
@@ -4341,6 +5108,10 @@
       <c r="D15" s="6" t="s">
         <v>498</v>
       </c>
+      <c r="E15">
+        <f t="shared" si="0"/>
+        <v>3013</v>
+      </c>
     </row>
     <row r="16" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B16" t="s">
@@ -4349,8 +5120,9 @@
       <c r="D16" s="6" t="s">
         <v>500</v>
       </c>
-      <c r="E16" t="s">
-        <v>482</v>
+      <c r="E16">
+        <f t="shared" si="0"/>
+        <v>3014</v>
       </c>
     </row>
     <row r="17" spans="2:5" ht="28.8" x14ac:dyDescent="0.3">
@@ -4363,6 +5135,10 @@
       <c r="D17" s="6" t="s">
         <v>502</v>
       </c>
+      <c r="E17">
+        <f t="shared" si="0"/>
+        <v>3015</v>
+      </c>
     </row>
     <row r="18" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B18" t="s">
@@ -4371,8 +5147,9 @@
       <c r="D18" s="6" t="s">
         <v>504</v>
       </c>
-      <c r="E18" t="s">
-        <v>482</v>
+      <c r="E18">
+        <f t="shared" si="0"/>
+        <v>3016</v>
       </c>
     </row>
     <row r="19" spans="2:5" x14ac:dyDescent="0.3">
@@ -4382,6 +5159,10 @@
       <c r="D19" s="6" t="s">
         <v>506</v>
       </c>
+      <c r="E19">
+        <f t="shared" si="0"/>
+        <v>3017</v>
+      </c>
     </row>
     <row r="20" spans="2:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B20" t="s">
@@ -4390,6 +5171,10 @@
       <c r="D20" s="6" t="s">
         <v>508</v>
       </c>
+      <c r="E20">
+        <f t="shared" si="0"/>
+        <v>3018</v>
+      </c>
     </row>
     <row r="21" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B21" t="s">
@@ -4401,8 +5186,9 @@
       <c r="D21" s="6" t="s">
         <v>510</v>
       </c>
-      <c r="E21" t="s">
-        <v>482</v>
+      <c r="E21">
+        <f t="shared" si="0"/>
+        <v>3019</v>
       </c>
     </row>
     <row r="22" spans="2:5" x14ac:dyDescent="0.3">
@@ -4415,8 +5201,9 @@
       <c r="D22" s="6" t="s">
         <v>512</v>
       </c>
-      <c r="E22" t="s">
-        <v>482</v>
+      <c r="E22">
+        <f t="shared" si="0"/>
+        <v>3020</v>
       </c>
     </row>
     <row r="23" spans="2:5" x14ac:dyDescent="0.3">
@@ -4429,8 +5216,15 @@
       <c r="D23" s="6" t="s">
         <v>514</v>
       </c>
-      <c r="E23" t="s">
-        <v>482</v>
+      <c r="E23">
+        <f t="shared" si="0"/>
+        <v>3021</v>
+      </c>
+    </row>
+    <row r="24" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="E24">
+        <f t="shared" si="0"/>
+        <v>3022</v>
       </c>
     </row>
     <row r="25" spans="2:5" ht="28.8" x14ac:dyDescent="0.3">
@@ -4443,6 +5237,10 @@
       <c r="D25" s="6" t="s">
         <v>516</v>
       </c>
+      <c r="E25">
+        <f t="shared" si="0"/>
+        <v>3023</v>
+      </c>
     </row>
     <row r="26" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B26" t="s">
@@ -4454,8 +5252,15 @@
       <c r="D26" s="6" t="s">
         <v>518</v>
       </c>
-      <c r="E26" t="s">
-        <v>482</v>
+      <c r="E26">
+        <f t="shared" si="0"/>
+        <v>3024</v>
+      </c>
+    </row>
+    <row r="27" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="E27">
+        <f t="shared" si="0"/>
+        <v>3025</v>
       </c>
     </row>
     <row r="28" spans="2:5" ht="43.2" x14ac:dyDescent="0.3">
@@ -4468,6 +5273,16 @@
       <c r="D28" s="6" t="s">
         <v>520</v>
       </c>
+      <c r="E28">
+        <f t="shared" si="0"/>
+        <v>3026</v>
+      </c>
+    </row>
+    <row r="29" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="E29">
+        <f t="shared" si="0"/>
+        <v>3027</v>
+      </c>
     </row>
     <row r="30" spans="2:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B30" t="s">
@@ -4476,6 +5291,10 @@
       <c r="D30" s="6" t="s">
         <v>522</v>
       </c>
+      <c r="E30">
+        <f t="shared" si="0"/>
+        <v>3028</v>
+      </c>
     </row>
     <row r="31" spans="2:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B31" t="s">
@@ -4487,8 +5306,9 @@
       <c r="D31" s="6" t="s">
         <v>524</v>
       </c>
-      <c r="E31" t="s">
-        <v>482</v>
+      <c r="E31">
+        <f t="shared" si="0"/>
+        <v>3029</v>
       </c>
     </row>
   </sheetData>
@@ -4527,7 +5347,7 @@
         <v>1</v>
       </c>
       <c r="E1" s="14" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
@@ -4732,7 +5552,7 @@
         <v>556</v>
       </c>
       <c r="D19" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="E19">
         <f t="shared" si="0"/>
@@ -4741,7 +5561,7 @@
     </row>
     <row r="20" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B20" s="2" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
       <c r="E20">
         <f t="shared" si="0"/>
@@ -4756,19 +5576,24 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{45C22DFD-A01D-4279-8877-CF35464686E2}">
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:K3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D34" sqref="D34"/>
+    <sheetView tabSelected="1" zoomScale="86" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2:H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="3" max="3" width="16.44140625" customWidth="1"/>
     <col min="4" max="4" width="19.5546875" customWidth="1"/>
+    <col min="6" max="6" width="25.21875" customWidth="1"/>
+    <col min="7" max="7" width="21" customWidth="1"/>
+    <col min="8" max="8" width="13.44140625" customWidth="1"/>
+    <col min="9" max="9" width="25" customWidth="1"/>
+    <col min="11" max="11" width="15.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="21" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" ht="24.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="14" t="s">
         <v>428</v>
       </c>
@@ -4782,10 +5607,28 @@
         <v>1</v>
       </c>
       <c r="E1" s="14" t="s">
-        <v>561</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+        <v>560</v>
+      </c>
+      <c r="F1" s="14" t="s">
+        <v>563</v>
+      </c>
+      <c r="G1" s="14" t="s">
+        <v>564</v>
+      </c>
+      <c r="H1" s="14" t="s">
+        <v>566</v>
+      </c>
+      <c r="I1" s="14" t="s">
+        <v>567</v>
+      </c>
+      <c r="J1" s="14" t="s">
+        <v>568</v>
+      </c>
+      <c r="K1" s="14" t="s">
+        <v>569</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
         <v>557</v>
       </c>
@@ -4796,12 +5639,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
         <v>559</v>
       </c>
       <c r="C3" t="s">
-        <v>560</v>
+        <v>565</v>
       </c>
       <c r="E3">
         <v>2</v>
@@ -4817,11 +5660,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{512EE97B-7681-4E1B-8C30-388F0DF91A75}">
   <dimension ref="A1:C42"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="3" max="3" width="80.6640625" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
@@ -5202,20 +6048,25 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <aa6b486ff96646b3bc945a43d61f9e88 xmlns="6f97b7b8-2b0e-4769-b7c4-80f9cf634925">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </aa6b486ff96646b3bc945a43d61f9e88>
-    <TaxCatchAll xmlns="6f97b7b8-2b0e-4769-b7c4-80f9cf634925" xsi:nil="true"/>
-    <a7ea6d49f3794e54851042dc4449d49f xmlns="6f97b7b8-2b0e-4769-b7c4-80f9cf634925">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </a7ea6d49f3794e54851042dc4449d49f>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<customXsn xmlns="http://schemas.microsoft.com/office/2006/metadata/customXsn">
+  <xsnLocation/>
+  <cached>True</cached>
+  <openByDefault>True</openByDefault>
+  <xsnScope/>
+</customXsn>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Excel spreadsheet" ma:contentTypeID="0x01011C0500EF85D2191EBEF3469FA6D2DA9B486D81" ma:contentTypeVersion="5" ma:contentTypeDescription="Itera templates 5" ma:contentTypeScope="" ma:versionID="a73035f95f634812d57091410501fcff">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="6f97b7b8-2b0e-4769-b7c4-80f9cf634925" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="cbd0edbc616daaf9aaf6ade75e5560a0" ns2:_="">
     <xsd:import namespace="6f97b7b8-2b0e-4769-b7c4-80f9cf634925"/>
@@ -5375,36 +6226,37 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<customXsn xmlns="http://schemas.microsoft.com/office/2006/metadata/customXsn">
-  <xsnLocation/>
-  <cached>True</cached>
-  <openByDefault>True</openByDefault>
-  <xsnScope/>
-</customXsn>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <aa6b486ff96646b3bc945a43d61f9e88 xmlns="6f97b7b8-2b0e-4769-b7c4-80f9cf634925">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </aa6b486ff96646b3bc945a43d61f9e88>
+    <TaxCatchAll xmlns="6f97b7b8-2b0e-4769-b7c4-80f9cf634925" xsi:nil="true"/>
+    <a7ea6d49f3794e54851042dc4449d49f xmlns="6f97b7b8-2b0e-4769-b7c4-80f9cf634925">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </a7ea6d49f3794e54851042dc4449d49f>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A8497EF5-02A1-4CA6-A9C6-F014DA66EE27}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{09B756EC-B2FD-4510-A6A4-DB36FE2E3D63}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="6f97b7b8-2b0e-4769-b7c4-80f9cf634925"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/customXsn"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{39989B6B-F442-4A18-8501-9CB5422E4AFE}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4BEB9EAD-FCDE-4F96-ACBB-61311D71BF01}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -5422,18 +6274,12 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{39989B6B-F442-4A18-8501-9CB5422E4AFE}">
+<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A8497EF5-02A1-4CA6-A9C6-F014DA66EE27}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{09B756EC-B2FD-4510-A6A4-DB36FE2E3D63}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/customXsn"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="6f97b7b8-2b0e-4769-b7c4-80f9cf634925"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>